<commit_message>
feature based docs p1
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C7B0B2-D885-4E8B-9D48-26BBB78CA8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE84A6B-73D5-4C70-A3BC-7FE8E81A9CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>HIVE-COTE 1.0</t>
   </si>
   <si>
-    <t>HICE-COTE 2.0</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>R-STSF</t>
+  </si>
+  <si>
+    <t>HIVE-COTE 2.0</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,37 +617,37 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
       <c r="M1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -676,43 +676,43 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -724,43 +724,43 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -772,43 +772,43 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -820,43 +820,43 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -892,43 +892,43 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -940,43 +940,43 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -988,43 +988,43 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1036,43 +1036,43 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1096,43 +1096,43 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1144,43 +1144,43 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1192,43 +1192,43 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1240,43 +1240,43 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1315,40 +1315,40 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1360,43 +1360,43 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1411,40 +1411,40 @@
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1480,43 +1480,43 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1528,43 +1528,43 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1576,43 +1576,43 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1624,43 +1624,43 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1672,43 +1672,43 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1720,43 +1720,43 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1795,40 +1795,40 @@
         <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -1843,40 +1843,40 @@
         <v>10</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -1914,40 +1914,40 @@
         <v>5</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -1962,40 +1962,40 @@
         <v>6</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -2034,40 +2034,40 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>

</xml_diff>

<commit_message>
tid v1, needs testing
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B34E444-C3B7-482B-A10A-138DBD2FCB87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462CE7E1-DA46-4C83-856A-1882ABD1D9B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
@@ -640,7 +640,7 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,8 +1791,8 @@
       <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="4" t="s">
-        <v>39</v>
+      <c r="M27" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1827,11 +1827,11 @@
       <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>39</v>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>16</v>
@@ -1839,8 +1839,8 @@
       <c r="L28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>39</v>
+      <c r="M28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>

</xml_diff>

<commit_message>
tde oob and docs, individualtde todo
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B34E444-C3B7-482B-A10A-138DBD2FCB87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3468507D-2916-485C-A55B-DB961A1741F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
+    <workbookView xWindow="-27495" yWindow="2820" windowWidth="16395" windowHeight="13155" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier Capabilities" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,8 +843,8 @@
       <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>39</v>
+      <c r="M5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1827,11 +1827,11 @@
       <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>39</v>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>16</v>
@@ -1839,8 +1839,8 @@
       <c r="L28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>39</v>
+      <c r="M28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1947,11 +1947,11 @@
       <c r="H31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>39</v>
+      <c r="I31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>16</v>
@@ -1959,8 +1959,8 @@
       <c r="L31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="4" t="s">
-        <v>39</v>
+      <c r="M31" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>

</xml_diff>

<commit_message>
DrCIF and CIF additions and documentation for HC2 (#1269)
* drcif contracting and train estimates

* tid start

* tid clean

* tid v1, needs testing

* CIF docs parameters and tags

* cif documentations. missing method docs

* CIT comments

* CIF check n_jobs

* CIF test refactor

* CIF example dataset change

* CIF comment space

* CIF faster tests

* test fixes

* wrong predict proba

Co-authored-by: Tony Bagnall <ajb@uea.ac.uk>
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B34E444-C3B7-482B-A10A-138DBD2FCB87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4064A349-0B02-4D70-97D2-12E8DBA7FC24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
@@ -188,9 +188,6 @@
     <t>MUSE</t>
   </si>
   <si>
-    <t>Not applicable for the classifier.</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Not present/Unsatisfactory</t>
+  </si>
+  <si>
+    <t>Not applicable for the classifier</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,8 +1791,8 @@
       <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="4" t="s">
-        <v>39</v>
+      <c r="M27" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1827,11 +1827,11 @@
       <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>39</v>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>16</v>
@@ -1839,8 +1839,8 @@
       <c r="L28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>39</v>
+      <c r="M28" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -2200,7 +2200,7 @@
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
@@ -2218,7 +2218,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -2246,7 +2246,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -2274,7 +2274,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>

</xml_diff>

<commit_message>
TDE additions and documentation for HC2 (#1357)
* TDE test updates

* tde refactor p1

* tde refactor p1

* parameter reformat

* tde oob and docs, individualtde todo

* histogram intersection docs

* individualtde refactor

* wront classifier name in test
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4064A349-0B02-4D70-97D2-12E8DBA7FC24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3468507D-2916-485C-A55B-DB961A1741F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
+    <workbookView xWindow="-27495" yWindow="2820" windowWidth="16395" windowHeight="13155" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier Capabilities" sheetId="1" r:id="rId1"/>
@@ -188,6 +188,9 @@
     <t>MUSE</t>
   </si>
   <si>
+    <t>Not applicable for the classifier.</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -195,9 +198,6 @@
   </si>
   <si>
     <t>Not present/Unsatisfactory</t>
-  </si>
-  <si>
-    <t>Not applicable for the classifier</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,8 +843,8 @@
       <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>39</v>
+      <c r="M5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1791,8 +1791,8 @@
       <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="5" t="s">
-        <v>16</v>
+      <c r="M27" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1947,11 +1947,11 @@
       <c r="H31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>39</v>
+      <c r="I31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>16</v>
@@ -1959,8 +1959,8 @@
       <c r="L31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="4" t="s">
-        <v>39</v>
+      <c r="M31" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -2200,7 +2200,7 @@
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
@@ -2218,7 +2218,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -2246,7 +2246,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -2274,7 +2274,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>

</xml_diff>

<commit_message>
experiments and arff reader
</commit_message>
<xml_diff>
--- a/sktime/contrib/classification_checklist.xlsx
+++ b/sktime/contrib/classification_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP Machine Learning\sktime-workshop-boss\sktime\contrib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DD2038-B91C-4F61-B27B-861A310ED0AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5B2E6D-ABD4-466F-9952-24754B2015C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
+    <workbookView xWindow="6210" yWindow="1035" windowWidth="16395" windowHeight="13155" xr2:uid="{3113605E-04EF-4EF3-A073-EC3617088A21}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier Capabilities" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE334DD-AE10-4914-BCE9-70451FC2855F}">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,8 +1467,8 @@
       <c r="H20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>16</v>
+      <c r="I20" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>16</v>

</xml_diff>